<commit_message>
update py code 08/29/2019
</commit_message>
<xml_diff>
--- a/gmail_flight.xlsx
+++ b/gmail_flight.xlsx
@@ -325,7 +325,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -355,12 +355,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>817</t>
+          <t>817 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>718</t>
+          <t>718 </t>
         </is>
       </c>
     </row>
@@ -372,12 +372,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>775</t>
+          <t>775 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>817</t>
+          <t>817 </t>
         </is>
       </c>
     </row>
@@ -389,12 +389,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>817</t>
+          <t>817 </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>775</t>
+          <t>775 </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed price and airline bugs
update re patterns to capture all cases of snippet
take prices from subject, if not available, go to snippet
</commit_message>
<xml_diff>
--- a/gmail_flight.xlsx
+++ b/gmail_flight.xlsx
@@ -322,10 +322,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D17"/>
+      <selection activeCell="A2" sqref="A2:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Multiple airlines</t>
+          <t>EVA cooperated</t>
         </is>
       </c>
     </row>
@@ -612,7 +612,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Your tracked</t>
+          <t>EVA cooperated</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,227 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Your tracked</t>
+          <t>EVA cooperated</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>09/28/19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>$1,301</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$1,147</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>EVA cooperated</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>09/29/19</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>$742</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$848</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Multiple airlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>09/30/19</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>$1,147</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$1,301</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>EVA cooperated</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>10/01/19</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>$878</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$742</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>EVA Air &amp; cooeperated</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>10/04/19</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$825</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$878</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Multiple airlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>10/05/19</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>$1,353</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$2,028</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>EVA Air</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10/06/19</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>$1,966</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$1,353</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>EVA Air</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10/07/19</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$2,520</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$1,966</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>EVA Air</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>10/08/19</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>$2,365</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$2,520</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>EVA Air</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>10/09/19</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>$757</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$825</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Multiple airlines</t>
         </is>
       </c>
     </row>

</xml_diff>